<commit_message>
Copyright, Domain + note(r) og Notex
</commit_message>
<xml_diff>
--- a/data-raw/metadata/metadata_BEXLTALL.xlsx
+++ b/data-raw/metadata/metadata_BEXLTALL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/672a29ec829a16e8/Dokumenter/GitHub/ProjCore/px/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{95AD3770-CFF6-4475-9029-B56B8E5608FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC43F236-33D2-4363-859F-1D3B58B40C84}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{95AD3770-CFF6-4475-9029-B56B8E5608FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95CC5B97-1342-4BFF-A4D8-E86C02E72A37}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables_MD" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="295">
   <si>
     <t>position</t>
   </si>
@@ -898,6 +898,15 @@
   </si>
   <si>
     <t>no of years</t>
+  </si>
+  <si>
+    <t>antal</t>
+  </si>
+  <si>
+    <t>amerlassusaat</t>
+  </si>
+  <si>
+    <t>FIGURES</t>
   </si>
 </sst>
 </file>
@@ -962,10 +971,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1289,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1545,6 +1550,23 @@
       </c>
       <c r="L8" t="s">
         <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C9" t="s">
+        <v>292</v>
+      </c>
+      <c r="D9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E9" t="s">
+        <v>293</v>
+      </c>
+      <c r="F9" t="s">
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -3603,7 +3625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
utf-8 to ANSI - additional package TAF
</commit_message>
<xml_diff>
--- a/data-raw/metadata/metadata_BEXLTALL.xlsx
+++ b/data-raw/metadata/metadata_BEXLTALL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/672a29ec829a16e8/Dokumenter/GitHub/ProjCore/px/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{79CCC2D3-1A8E-44B3-94BD-6033C059658E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADC63F4B-5784-4EC3-BA17-4AD0BABB5A2B}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{79CCC2D3-1A8E-44B3-94BD-6033C059658E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB47A784-CBF9-4162-97DF-259F84945E4E}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables_MD" sheetId="1" r:id="rId1"/>
@@ -828,9 +828,6 @@
     <t>CHARSET</t>
   </si>
   <si>
-    <t>utf-8</t>
-  </si>
-  <si>
     <t>AXIS_VERSION</t>
   </si>
   <si>
@@ -877,6 +874,9 @@
   </si>
   <si>
     <t>20230222 09:00</t>
+  </si>
+  <si>
+    <t>ANSI</t>
   </si>
 </sst>
 </file>
@@ -944,10 +944,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1399,7 +1395,7 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -1495,7 +1491,7 @@
         <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D7" t="s">
         <v>47</v>
@@ -1550,16 +1546,16 @@
         <v>193</v>
       </c>
       <c r="C9" t="s">
+        <v>280</v>
+      </c>
+      <c r="D9" t="s">
+        <v>280</v>
+      </c>
+      <c r="E9" t="s">
         <v>281</v>
       </c>
-      <c r="D9" t="s">
-        <v>281</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>282</v>
-      </c>
-      <c r="F9" t="s">
-        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -1571,8 +1567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="H101" sqref="H101"/>
+    <sheetView topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3932,8 +3928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3954,12 +3950,12 @@
         <v>267</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B3" s="2">
         <v>2000</v>
@@ -3967,26 +3963,26 @@
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" t="s">
         <v>270</v>
-      </c>
-      <c r="B4" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>271</v>
+      </c>
+      <c r="B5" t="s">
         <v>272</v>
-      </c>
-      <c r="B5" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B6" t="s">
         <v>274</v>
-      </c>
-      <c r="B6" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -4183,7 +4179,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B31" t="s">
         <v>231</v>
@@ -4194,12 +4190,12 @@
         <v>232</v>
       </c>
       <c r="B32" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B33">
         <v>15</v>
@@ -4207,7 +4203,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B34">
         <v>0</v>

</xml_diff>